<commit_message>
ajout des classes et debut de la conception de la fiche de personnage
</commit_message>
<xml_diff>
--- a/Regles et tableau/Classes/Classe maitre/Chasseur de trésor.xlsx
+++ b/Regles et tableau/Classes/Classe maitre/Chasseur de trésor.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>Rôle au sein du groupe</t>
   </si>
@@ -113,13 +113,37 @@
   </si>
   <si>
     <t>Chasseur de trésor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les tests de fouilles sont automatiquement réussi (sauf échec critique). La marge de critique est maintenant de 18-20. Le chasseur de trésor dispose d'un dé </t>
+  </si>
+  <si>
+    <t>d'action gratuit par scène pour réaliser un test de fouille.</t>
+  </si>
+  <si>
+    <t>Le chasseur de trésor peut relancer chaque DD de butin une fois.</t>
+  </si>
+  <si>
+    <t>A chaque combat, le chasseur de trésor gagne un butin d'équipement et de magie avec un modificateur de +5.</t>
+  </si>
+  <si>
+    <t>Pour chaque trésor de scène, si le chasseur de trésor réussi un test critique de fouille, le groupe trouve un trésor supplémentaire.</t>
+  </si>
+  <si>
+    <t>A chaque réussite critique de fouille, le chasseur de trésor gagne un Butin PA et au choix un équipement ou magie. Pour chaque DD de butin supérieur à 40/50, le chasseur</t>
+  </si>
+  <si>
+    <t>de trésor gagne un butin supplémentaire du même type.</t>
+  </si>
+  <si>
+    <t>Le chasseur de trésor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +169,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="25"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -186,19 +217,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -506,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:S17"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,380 +553,601 @@
     <col min="1" max="1" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+    </row>
     <row r="4" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
     </row>
     <row r="8" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
     </row>
     <row r="10" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
     </row>
     <row r="13" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
     </row>
     <row r="14" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
     </row>
     <row r="15" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
     </row>
     <row r="16" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-    </row>
-    <row r="17" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+    </row>
+    <row r="17" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+    </row>
+    <row r="20" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+    </row>
+    <row r="21" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+    </row>
+    <row r="22" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+    </row>
+    <row r="23" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+    </row>
+    <row r="24" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+    </row>
+    <row r="25" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+    </row>
+    <row r="26" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="H12:S12"/>
-    <mergeCell ref="H13:S13"/>
+  <mergeCells count="19">
     <mergeCell ref="H14:S14"/>
     <mergeCell ref="H15:S15"/>
     <mergeCell ref="H16:S16"/>
+    <mergeCell ref="B24:S24"/>
+    <mergeCell ref="B26:S26"/>
+    <mergeCell ref="A1:S2"/>
+    <mergeCell ref="B20:S20"/>
+    <mergeCell ref="B21:S21"/>
+    <mergeCell ref="B22:S22"/>
+    <mergeCell ref="B23:S23"/>
     <mergeCell ref="H17:S17"/>
     <mergeCell ref="B4:S4"/>
     <mergeCell ref="B5:S5"/>
@@ -898,6 +1155,8 @@
     <mergeCell ref="B7:S7"/>
     <mergeCell ref="B8:S8"/>
     <mergeCell ref="B10:S10"/>
+    <mergeCell ref="H12:S12"/>
+    <mergeCell ref="H13:S13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>